<commit_message>
Doing the finishing touch with these lines.
</commit_message>
<xml_diff>
--- a/Hours_sum.xlsx
+++ b/Hours_sum.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User\Tantargyak\Projlab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User\Tantargyak\Projlab\zeta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0DFB00E-B877-4037-9F5B-48C34A7DF756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA0088D-A608-4C46-8D2C-4C8FB5AF9EE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4B684547-BE2B-4ADD-BF32-A5297FD40BB1}"/>
   </bookViews>
@@ -514,11 +514,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7B4D1FD-FBCC-48DF-AE99-9DBE657AB48B}">
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F64" sqref="F64"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1195,7 +1195,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="12">
         <v>60</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
       <c r="B50" s="11">
         <v>1800</v>
@@ -1217,7 +1217,7 @@
       <c r="D50" s="1"/>
       <c r="E50" s="6"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
       <c r="B51" s="11">
         <v>90</v>
@@ -1228,7 +1228,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
       <c r="B52" s="11">
         <v>140</v>
@@ -1239,7 +1239,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
       <c r="B53" s="11">
         <v>90</v>
@@ -1250,7 +1250,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>360</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="7">
         <v>60</v>
       </c>
@@ -1280,56 +1280,112 @@
       </c>
       <c r="E55" s="9"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
-        <f>SUM(A2:A55)</f>
-        <v>8600</v>
-      </c>
-      <c r="B56">
-        <f t="shared" ref="B56:E56" si="0">SUM(B2:B55)</f>
-        <v>11120</v>
+        <v>60</v>
+      </c>
+      <c r="B56" s="11">
+        <v>60</v>
       </c>
       <c r="C56">
+        <v>60</v>
+      </c>
+      <c r="D56">
+        <v>60</v>
+      </c>
+      <c r="E56" s="16">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>120</v>
+      </c>
+      <c r="B57" s="11">
+        <v>60</v>
+      </c>
+      <c r="C57">
+        <v>60</v>
+      </c>
+      <c r="D57">
+        <v>240</v>
+      </c>
+      <c r="E57" s="16">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>180</v>
+      </c>
+      <c r="B58" s="11">
+        <v>2400</v>
+      </c>
+      <c r="C58">
+        <v>1800</v>
+      </c>
+      <c r="D58">
+        <v>3600</v>
+      </c>
+      <c r="E58" s="16">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B59" s="11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <f>SUM(A2:A58)</f>
+        <v>8960</v>
+      </c>
+      <c r="B65">
+        <f>SUM(B2:B59)</f>
+        <v>13700</v>
+      </c>
+      <c r="C65">
+        <f>SUM(C2:C58)</f>
+        <v>10170</v>
+      </c>
+      <c r="D65">
+        <f>SUM(D2:D58)</f>
+        <v>13460</v>
+      </c>
+      <c r="E65">
+        <f>SUM(E2:E58)</f>
+        <v>5510</v>
+      </c>
+      <c r="F65">
+        <f>SUM(A65:E65)</f>
+        <v>51800</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="str">
+        <f xml:space="preserve"> (INT(A65/60)) &amp; " óra " &amp; ROUND((((A65/60)-INT(A65/60))*60),0) &amp; " perc"</f>
+        <v>149 óra 20 perc</v>
+      </c>
+      <c r="B68" t="str">
+        <f t="shared" ref="B68:F68" si="0" xml:space="preserve"> (INT(B65/60)) &amp; " óra " &amp; ROUND((((B65/60)-INT(B65/60))*60),0) &amp; " perc"</f>
+        <v>228 óra 20 perc</v>
+      </c>
+      <c r="C68" t="str">
         <f t="shared" si="0"/>
-        <v>8250</v>
-      </c>
-      <c r="D56">
+        <v>169 óra 30 perc</v>
+      </c>
+      <c r="D68" t="str">
         <f t="shared" si="0"/>
-        <v>9560</v>
-      </c>
-      <c r="E56">
+        <v>224 óra 20 perc</v>
+      </c>
+      <c r="E68" t="str">
         <f t="shared" si="0"/>
-        <v>3950</v>
-      </c>
-      <c r="F56">
-        <f>SUM(A56:E56)</f>
-        <v>41480</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" t="str">
-        <f xml:space="preserve"> (INT(A56/60)) &amp; " óra " &amp; ROUND((((A56/60)-INT(A56/60))*60),0) &amp; " perc"</f>
-        <v>143 óra 20 perc</v>
-      </c>
-      <c r="B59" t="str">
-        <f t="shared" ref="B59:F59" si="1" xml:space="preserve"> (INT(B56/60)) &amp; " óra " &amp; ROUND((((B56/60)-INT(B56/60))*60),0) &amp; " perc"</f>
-        <v>185 óra 20 perc</v>
-      </c>
-      <c r="C59" t="str">
-        <f t="shared" si="1"/>
-        <v>137 óra 30 perc</v>
-      </c>
-      <c r="D59" t="str">
-        <f t="shared" si="1"/>
-        <v>159 óra 20 perc</v>
-      </c>
-      <c r="E59" t="str">
-        <f t="shared" si="1"/>
-        <v>65 óra 50 perc</v>
-      </c>
-      <c r="F59" t="str">
-        <f t="shared" si="1"/>
-        <v>691 óra 20 perc</v>
+        <v>91 óra 50 perc</v>
+      </c>
+      <c r="F68" t="str">
+        <f t="shared" si="0"/>
+        <v>863 óra 20 perc</v>
       </c>
     </row>
   </sheetData>

</xml_diff>